<commit_message>
Versão 1.0 de DRI
</commit_message>
<xml_diff>
--- a/02-PROJETO-2015.2/01-GERENCIA DE PROJETO/DRI-Documento de Riscos.xlsx
+++ b/02-PROJETO-2015.2/01-GERENCIA DE PROJETO/DRI-Documento de Riscos.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Tabela_de_severidade" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Ação">Planilha_de_Riscos!$J$5:$J$65349</definedName>
+    <definedName name="Ação">Planilha_de_Riscos!$J$5:$J$65351</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="114">
   <si>
     <t>PLANILHA DE RISCOS</t>
   </si>
@@ -293,9 +293,6 @@
     <t>Indisponibilidade dos Clientes</t>
   </si>
   <si>
-    <t>Necessidade de Utilização de Nova Tecnologia Desconhecida pela Equipe</t>
-  </si>
-  <si>
     <t>Desistência de um Membro da Equipe</t>
   </si>
   <si>
@@ -330,9 +327,6 @@
   </si>
   <si>
     <t>Falha do Planejamento Inicial do Projeto</t>
-  </si>
-  <si>
-    <t>Aumento de Complexidade, modificação em escopo inicialmente planejado</t>
   </si>
   <si>
     <r>
@@ -411,7 +405,482 @@
     <t>Negativo</t>
   </si>
   <si>
-    <t>Recursos de Hardware e Softwares Indisponíveis</t>
+    <r>
+      <t xml:space="preserve">Provável atraso nas próximas iterações, em entregas de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>releases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ao cliente e na finalização do projeto, baixa qualidade do produto final.</t>
+    </r>
+  </si>
+  <si>
+    <t>Falha na identificação e no planejamento da mitigação dos riscos.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Baixa qualidade da </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>release</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e consequentemente, insatisfação do cliente, reclamações e retrabalhos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Recursos (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Hardware </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Softwares</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) Indisponíveis</t>
+    </r>
+  </si>
+  <si>
+    <t>Atraso, ou até não entrega, de sistema.</t>
+  </si>
+  <si>
+    <t>Aumento de escopo iteração atual, aumento de custo referente a disponibilização de tempo.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Planejamento inicial atrasado ou mau elaborado, falta de opnião sobre satisfação de item de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>backlog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Aumento de complexidade de sistema, modificação em escopo inicialmente planejado, aumento de trabalho.</t>
+  </si>
+  <si>
+    <t>Mudança em escopos de iterações já planejadas, provável atraso na finalização de iterações devido o aumento do escopo.</t>
+  </si>
+  <si>
+    <t>Aumento de escopo de iterações e, consequentemente, atrasos na entrega, baixa qualidade do produto.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sobrecarga de trabalho para membro restante, atraso em entregas de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>releases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, itens de backlog e produto final, provável baixa qualidade em entregas.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sobrecarga de trabalho para membro restante, provável atraso ou não finalização de iteração, provável baixa qualidade em entregas.</t>
+  </si>
+  <si>
+    <t>Atraso de iteração ou inviabilização de funcionalidade referente ao login.</t>
+  </si>
+  <si>
+    <t>Falha no gerenciamento de iteração.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dificuldades na identificação de falhas na </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>build</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do projeto.</t>
+    </r>
+  </si>
+  <si>
+    <t>Técnico</t>
+  </si>
+  <si>
+    <t>Gerenciamento de Projetos</t>
+  </si>
+  <si>
+    <t>Organizacional</t>
+  </si>
+  <si>
+    <t>Externo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Metas de desempenhos irreais, atrasos em entrega de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>releases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, falha na identificação e mitigação de riscos, papéis e stakeholders mau definidos, dispersão na definição da arquitetura do sistema, baixa qualidade do produto final.</t>
+    </r>
+  </si>
+  <si>
+    <t>Má Distribuição de Tempo nas Atividades da Iteração</t>
+  </si>
+  <si>
+    <t>Atraso ou não finalização de entrega da iteração, provável baixa de qualidade causada pela falta de testes.</t>
+  </si>
+  <si>
+    <t>Dificuldade de Comunicação entre Membros de Equipe</t>
+  </si>
+  <si>
+    <t>Retrabalho, insconsistência em trabalho produzido.</t>
+  </si>
+  <si>
+    <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
+  </si>
+  <si>
+    <t>Aceitar</t>
+  </si>
+  <si>
+    <t>Aberto</t>
+  </si>
+  <si>
+    <t>Equipe de Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Líder de Projeto</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Necessidade de Utilização para Nova Tecnologia não Planejada pela Equipe</t>
+  </si>
+  <si>
+    <t>Atrasos em iterações, mau uso de tecnologia devido a falta de tempo.</t>
+  </si>
+  <si>
+    <t>Gerente de Configuração</t>
+  </si>
+  <si>
+    <t>Líder do Projeto</t>
+  </si>
+  <si>
+    <t>Link de ferramenta fora do ar.</t>
+  </si>
+  <si>
+    <t>Desistência do curso de algum membro da equipe.</t>
+  </si>
+  <si>
+    <t>Deslocamento dos membros da equipe para sua cidade natal.</t>
+  </si>
+  <si>
+    <t>Algum membro da equipe ser infectado por Zica, Denge ou Chikungunya.</t>
+  </si>
+  <si>
+    <t>Participação de algum membro da equipe de eventos da área de TI.</t>
+  </si>
+  <si>
+    <t>Utilização de nova ferramenta dificultada por baixa quantidade de documentação da mesma.</t>
+  </si>
+  <si>
+    <t>Inserção de nova ferrramenta não planejada pela equipe durante a ocorrência de uma iteração.</t>
+  </si>
+  <si>
+    <t>Cliente solicitar mudança por conta de novo regimento no Campus.</t>
+  </si>
+  <si>
+    <t>Entrada de novo Stakeholder.</t>
+  </si>
+  <si>
+    <t>Cliente se ausenta do Campus por motivos pessoais, profissionais ou de saúde.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testes em </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mal realizados.</t>
+    </r>
+  </si>
+  <si>
+    <t>Máquina de algum membro da equipe de desenvolvimento apresenta problemas.</t>
+  </si>
+  <si>
+    <t>Líder de projeto não planeja da melhor forma a iteração.</t>
+  </si>
+  <si>
+    <t>Líder de projeto não identifica todos os riscos possíveis no projeto.</t>
+  </si>
+  <si>
+    <t>Equipe de desenvolvimento não possui o tempo livre suficiente para finalização de iteração.</t>
+  </si>
+  <si>
+    <t>Líder de projeto não elabora de forma íntegra o planejamento do projeto.</t>
+  </si>
+  <si>
+    <t>Deslocamento das atividades para os membros restantes, buscar substituto, redefinir escopo.</t>
+  </si>
+  <si>
+    <t>Realização de análise para verificar se é possível adicionar fases pendentes a alguma iteração posterior.</t>
+  </si>
+  <si>
+    <t>Buscar erradicação de falha o mais cedo possível afim de evitar transtornos maiores.</t>
+  </si>
+  <si>
+    <t>Verificar a possibilidade de realização da iteração em tempo hábil, e caso seja impossível, replanejar itens para próxima iteração.</t>
+  </si>
+  <si>
+    <t>Concluir o mais cedo possível análise e inserir, caso seja preciso, os novos riscos no planejamento.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar viabilidade de realização de testes em iteração posterior afim de manter a qualidade do item de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">backlog </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>produzido.</t>
+    </r>
+  </si>
+  <si>
+    <t>Configurar máquina de laboratório para uso no desenvolvimento.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Analisar a viabilidade de correção de erros que surgiram em </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>disponibilida a cliente na iteração atual sem prejudicar próxima entrega.</t>
+    </r>
+  </si>
+  <si>
+    <t>Manter contatos atualizados de clientes afim de contatá-los de forma não presencial.</t>
+  </si>
+  <si>
+    <t>Analisar alteração de escopo e tempo, notificar cliente sobre consequências e implementá-las caso sejam viabilizadas.</t>
+  </si>
+  <si>
+    <t>Planejar horário fora do planejado para iteração com o intuíto de estudar sobre a ferramenta, mantendo a entrega ainda dentro dos parâmetros.</t>
+  </si>
+  <si>
+    <t>Verificar a possibilidade de troca de ferramenta sem que a entrega seja afetada.</t>
+  </si>
+  <si>
+    <t>Buscar erradicação de risco ainda no planejamento de iteração, afim de realizar planejamento de iteração com menos tempo disponível.</t>
+  </si>
+  <si>
+    <t>Realizar atividades planejadas de forma remota.</t>
+  </si>
+  <si>
+    <t>Gerar, sempre que passível de atenção, arquivo .pdf com atividades atualizadas da ferramenta.</t>
+  </si>
+  <si>
+    <t>Deslocar responsabilidade de verificação para algum membro da equipe.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reorganizar escopo de iteração, afim de aguardar, em casos de ferramenta fora do ar, correção de problema e avaliar, em casos da inviabilização de entrega do item de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">backlog, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>renegociação com cliente sobre entrega de requisito.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -983,7 +1452,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1009,9 +1478,104 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="18" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1021,98 +1585,6 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="18" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="104">
     <cellStyle name="cf1" xfId="1"/>
@@ -1677,10 +2149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1703,806 +2175,1246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17.850000000000001" customHeight="1">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:13" ht="14.1" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="15.2" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="25"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="38"/>
     </row>
     <row r="4" spans="1:13" ht="16.7" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="41"/>
     </row>
     <row r="5" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="44"/>
+      <c r="C6" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" ht="17.850000000000001" customHeight="1">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="17.850000000000001" customHeight="1">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" ht="17.850000000000001" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A11" s="30">
+    <row r="11" spans="1:13" s="2" customFormat="1" ht="38.25">
+      <c r="A11" s="14">
         <v>1</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="44"/>
-    </row>
-    <row r="12" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A12" s="30">
+      <c r="B11" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" ht="63.75">
+      <c r="A12" s="14">
         <f>A11+1</f>
         <v>2</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="30" customFormat="1" ht="51">
+      <c r="A13" s="14">
+        <f>A12+1</f>
+        <v>3</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" ht="38.25">
+      <c r="A14" s="14">
+        <f>A13+1</f>
+        <v>4</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="44"/>
-    </row>
-    <row r="13" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A13" s="30">
-        <f t="shared" ref="A13:A28" si="0">A12+1</f>
-        <v>3</v>
-      </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="44"/>
-    </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A14" s="30">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="44"/>
-    </row>
-    <row r="15" spans="1:13" s="46" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A15" s="30">
-        <f t="shared" si="0"/>
+      <c r="F14" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" ht="38.25">
+      <c r="A15" s="14">
+        <f t="shared" ref="A15:A30" si="0">A14+1</f>
         <v>5</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="45" t="s">
+      <c r="B15" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="44"/>
-    </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A16" s="30">
+      <c r="F15" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="L15" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="30" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A16" s="14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="41" t="s">
+      <c r="B16" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="44"/>
-    </row>
-    <row r="17" spans="1:13" s="46" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A17" s="30">
+      <c r="D16" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="L16" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" ht="38.25">
+      <c r="A17" s="14">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="44"/>
-    </row>
-    <row r="18" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A18" s="30">
+      <c r="B17" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="30" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A18" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="44"/>
-    </row>
-    <row r="19" spans="1:13" s="46" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A19" s="30">
+      <c r="B18" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="2" customFormat="1" ht="38.25">
+      <c r="A19" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="44"/>
-    </row>
-    <row r="20" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A20" s="30">
-        <f t="shared" si="0"/>
+      <c r="B19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J19" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="30" customFormat="1" ht="38.25">
+      <c r="A20" s="14">
+        <f>A19+1</f>
         <v>10</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="44"/>
-    </row>
-    <row r="21" spans="1:13" s="46" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A21" s="30">
-        <f t="shared" si="0"/>
+      <c r="B20" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="2" customFormat="1" ht="51">
+      <c r="A21" s="14">
+        <f>A20+1</f>
         <v>11</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="44"/>
-    </row>
-    <row r="22" spans="1:13" s="46" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A22" s="30">
+      <c r="B21" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="L21" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="30" customFormat="1" ht="38.25">
+      <c r="A22" s="14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="45" t="s">
+      <c r="B22" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="44"/>
-    </row>
-    <row r="23" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A23" s="30">
+      <c r="E22" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M22" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="30" customFormat="1" ht="51">
+      <c r="A23" s="14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="45" t="s">
+      <c r="B23" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="44"/>
-    </row>
-    <row r="24" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A24" s="30">
+      <c r="E23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="2" customFormat="1" ht="51">
+      <c r="A24" s="14">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="44"/>
-    </row>
-    <row r="25" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A25" s="30">
-        <f t="shared" si="0"/>
+      <c r="B24" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M24" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="30" customFormat="1" ht="25.5">
+      <c r="A25" s="14">
+        <f>A24+1</f>
         <v>15</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="45"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="44"/>
-    </row>
-    <row r="26" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A26" s="30">
-        <f t="shared" si="0"/>
+      <c r="B25" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M25" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="2" customFormat="1" ht="51">
+      <c r="A26" s="14">
+        <f>A25+1</f>
         <v>16</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="44"/>
-    </row>
-    <row r="27" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A27" s="30">
+      <c r="B26" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M26" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="2" customFormat="1" ht="76.5">
+      <c r="A27" s="14">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="44"/>
-    </row>
-    <row r="28" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A28" s="30">
+      <c r="B27" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M27" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="2" customFormat="1" ht="76.5">
+      <c r="A28" s="14">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="39"/>
-    </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="32"/>
-    </row>
-    <row r="30" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="36"/>
-    </row>
-    <row r="31" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="36"/>
+      <c r="B28" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="L28" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M28" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A29" s="14">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="L29" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="M29" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="2" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A30" s="14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L30" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="M30" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="16"/>
     </row>
     <row r="32" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="36"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="20"/>
     </row>
     <row r="33" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="36"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="20"/>
     </row>
     <row r="34" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="36"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="20"/>
     </row>
     <row r="35" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="36"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="20"/>
     </row>
     <row r="36" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A36" s="34"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="36"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="20"/>
     </row>
     <row r="37" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="36"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="20"/>
     </row>
     <row r="38" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A38" s="34"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="36"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="20"/>
     </row>
     <row r="39" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A39" s="34"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="36"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="20"/>
     </row>
     <row r="40" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="36"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="20"/>
     </row>
     <row r="41" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A41" s="34"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="36"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="20"/>
     </row>
     <row r="42" spans="1:13" ht="28.35" customHeight="1">
-      <c r="A42" s="34"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="37"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="36"/>
-    </row>
-    <row r="43" spans="1:13" ht="49.15" customHeight="1"/>
-    <row r="44" spans="1:13" ht="49.15" customHeight="1"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="20"/>
+    </row>
+    <row r="43" spans="1:13" ht="28.35" customHeight="1">
+      <c r="A43" s="18"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="20"/>
+    </row>
+    <row r="44" spans="1:13" ht="28.35" customHeight="1">
+      <c r="A44" s="18"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="20"/>
+    </row>
     <row r="45" spans="1:13" ht="49.15" customHeight="1"/>
     <row r="46" spans="1:13" ht="49.15" customHeight="1"/>
     <row r="47" spans="1:13" ht="49.15" customHeight="1"/>
@@ -2545,6 +3457,8 @@
     <row r="84" ht="49.15" customHeight="1"/>
     <row r="85" ht="49.15" customHeight="1"/>
     <row r="86" ht="49.15" customHeight="1"/>
+    <row r="87" ht="49.15" customHeight="1"/>
+    <row r="88" ht="49.15" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:B4"/>
@@ -2558,77 +3472,83 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:M8"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F42">
+  <conditionalFormatting sqref="F11:F44">
     <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H42">
+  <conditionalFormatting sqref="H11:H44">
     <cfRule type="cellIs" dxfId="14" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G42">
+  <conditionalFormatting sqref="G11:G44">
     <cfRule type="cellIs" dxfId="13" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Alto"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:F42">
+  <conditionalFormatting sqref="F11:F44">
     <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H42">
+  <conditionalFormatting sqref="H11:H44">
     <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G42">
+  <conditionalFormatting sqref="G11:G44">
     <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Baixo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:F42">
+  <conditionalFormatting sqref="F11:F44">
     <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H42">
+  <conditionalFormatting sqref="H11:H44">
     <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G42">
+  <conditionalFormatting sqref="G11:G44">
     <cfRule type="cellIs" dxfId="7" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Médio"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C42">
+  <conditionalFormatting sqref="C11:C44">
     <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Negativo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C42">
+  <conditionalFormatting sqref="C11:C44">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Positivo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" prompt="Mitigar_x000a_Aceitar_x000a_Transferir_x000a_Evitar" sqref="J43:J86"/>
-    <dataValidation type="list" allowBlank="1" sqref="C11:C42">
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Mitigar_x000a_Aceitar_x000a_Transferir_x000a_Evitar" sqref="J45:J88"/>
+    <dataValidation type="list" allowBlank="1" sqref="C11:C44">
       <formula1>"Positivo,Negativo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F11:F42">
+    <dataValidation type="list" allowBlank="1" sqref="F11:F44">
       <formula1>"Baixa,Média,Alta"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G11:G42">
+    <dataValidation type="list" allowBlank="1" sqref="G11:G44">
       <formula1>"Baixo,Médio,Alto"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I11:I42">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I11:I44">
       <formula1>"Aceitar,Mitigar,Eliminar,Transferir,Explorar,Compartilhar,Melhorar"</formula1>
     </dataValidation>
-    <dataValidation type="list" showErrorMessage="1" sqref="M11:M42">
+    <dataValidation type="list" showErrorMessage="1" sqref="M11:M44">
       <formula1>"Aberto,Fechado,Em Andamento"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B30">
+      <formula1>"Técnico,Externo,Organizacional,Gerenciamento de Projetos"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11:H30">
+      <formula1>"Baixa,Média,Alta"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.24370078740157503" right="0.24291338582677208" top="0.85236220472440904" bottom="0.48858267716535408" header="0.45826771653543297" footer="9.4488188976378021E-2"/>
@@ -2647,7 +3567,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2658,25 +3578,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" ht="26.45" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
     </row>
     <row r="3" spans="1:5" ht="44.45" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="4"/>
@@ -2691,7 +3611,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="44.45" customHeight="1">
-      <c r="A4" s="14"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2706,7 +3626,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="38.65" customHeight="1">
-      <c r="A5" s="14"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
@@ -2721,7 +3641,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="38.65" customHeight="1">
-      <c r="A6" s="14"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="10" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
VErsão 1.1 de ARQ e Versão 1.1 de DRI
</commit_message>
<xml_diff>
--- a/02-PROJETO-2015.2/01-GERENCIA DE PROJETO/DRI-Documento de Riscos.xlsx
+++ b/02-PROJETO-2015.2/01-GERENCIA DE PROJETO/DRI-Documento de Riscos.xlsx
@@ -2151,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Início de Iteração 03
</commit_message>
<xml_diff>
--- a/02-PROJETO-2015.2/01-GERENCIA DE PROJETO/DRI-Documento de Riscos.xlsx
+++ b/02-PROJETO-2015.2/01-GERENCIA DE PROJETO/DRI-Documento de Riscos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha_de_Riscos" sheetId="1" state="visible" r:id="rId2"/>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="118">
   <si>
     <t>SISTEMA DE GERENCIAMENTO DA ASSISTÊNCIA ESTUDANTIL</t>
   </si>
@@ -293,7 +293,6 @@
   <si>
     <r>
       <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -310,50 +309,39 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>releases</t>
+      <t>releases ao cliente e na finalização do projeto, baixa qualidade do produto final.</t>
     </r>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Equipe de desenvolvimento não possui o tempo livre suficiente para finalização de iteração.</t>
+  </si>
+  <si>
+    <t>Realizar amplo planejamento e cumprir prazos planejados</t>
+  </si>
+  <si>
+    <t>Equipe de Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Aberto</t>
+  </si>
+  <si>
+    <t>Gerenciamento de Projetos</t>
+  </si>
+  <si>
+    <t>Falha do Planejamento Inicial do Projeto</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> ao cliente e na finalização do projeto, baixa qualidade do produto final.</t>
-    </r>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Alto</t>
-  </si>
-  <si>
-    <t>Mitigar</t>
-  </si>
-  <si>
-    <t>Equipe de desenvolvimento não possui o tempo livre suficiente para finalização de iteração.</t>
-  </si>
-  <si>
-    <t>Realizar amplo planejamento e cumprir prazos planejados</t>
-  </si>
-  <si>
-    <t>Equipe de Desenvolvimento</t>
-  </si>
-  <si>
-    <t>Aberto</t>
-  </si>
-  <si>
-    <t>Gerenciamento de Projetos</t>
-  </si>
-  <si>
-    <t>Falha do Planejamento Inicial do Projeto</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -370,68 +358,57 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>releases</t>
+      <t>releases, falha na identificação e mitigação de riscos, papéis e stakeholders mau definidos, dispersão na definição da arquitetura do sistema, baixa qualidade do produto final.</t>
     </r>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Líder de projeto não elabora de forma íntegra o planejamento do projeto.</t>
+  </si>
+  <si>
+    <t>Realizar planejamento em tempo hábil e abragir maior quantidade de problemas e riscos possíveis.</t>
+  </si>
+  <si>
+    <t>Líder de Projeto</t>
+  </si>
+  <si>
+    <t>Má Distribuição de Tempo nas Atividades da Iteração</t>
+  </si>
+  <si>
+    <t>Atraso ou não finalização de entrega da iteração, provável baixa de qualidade causada pela falta de testes.</t>
+  </si>
+  <si>
+    <t>Médio</t>
+  </si>
+  <si>
+    <t>Líder de projeto não planeja da melhor forma a iteração.</t>
+  </si>
+  <si>
+    <t>Análise aprofudada de como devem ser realizadas tais atividades levantando o tempo e esforço necessários para a realização das mesmas.</t>
+  </si>
+  <si>
+    <t>Análise de Riscos Incompleta</t>
+  </si>
+  <si>
+    <t>Falha na identificação e no planejamento da mitigação dos riscos.</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
+  </si>
+  <si>
+    <t>Líder de projeto não identifica todos os riscos possíveis no projeto.</t>
+  </si>
+  <si>
+    <t>Concluir o mais cedo possível análise dos riscos.</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>, falha na identificação e mitigação de riscos, papéis e stakeholders mau definidos, dispersão na definição da arquitetura do sistema, baixa qualidade do produto final.</t>
-    </r>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Líder de projeto não elabora de forma íntegra o planejamento do projeto.</t>
-  </si>
-  <si>
-    <t>Realizar planejamento em tempo hábil e abragir maior quantidade de problemas e riscos possíveis.</t>
-  </si>
-  <si>
-    <t>Líder de Projeto</t>
-  </si>
-  <si>
-    <t>Má Distribuição de Tempo nas Atividades da Iteração</t>
-  </si>
-  <si>
-    <t>Atraso ou não finalização de entrega da iteração, provável baixa de qualidade causada pela falta de testes.</t>
-  </si>
-  <si>
-    <t>Médio</t>
-  </si>
-  <si>
-    <t>Líder de projeto não planeja da melhor forma a iteração.</t>
-  </si>
-  <si>
-    <t>Análise aprofudada de como devem ser realizadas tais atividades levantando o tempo e esforço necessários para a realização das mesmas.</t>
-  </si>
-  <si>
-    <t>Análise de Riscos Incompleta</t>
-  </si>
-  <si>
-    <t>Falha na identificação e no planejamento da mitigação dos riscos.</t>
-  </si>
-  <si>
-    <t>Baixa</t>
-  </si>
-  <si>
-    <t>Eliminar</t>
-  </si>
-  <si>
-    <t>Líder de projeto não identifica todos os riscos possíveis no projeto.</t>
-  </si>
-  <si>
-    <t>Concluir o mais cedo possível análise dos riscos.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -448,23 +425,12 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Release </t>
+      <t>Release de Iteração</t>
     </r>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>de Iteração</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -481,29 +447,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>release</t>
+      <t>release e consequentemente, insatisfação do cliente, reclamações e retrabalhos.</t>
     </r>
+  </si>
+  <si>
+    <t>Desenvolver testes gradativamente durante a iteração.</t>
+  </si>
+  <si>
+    <t>Organizacional</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> e consequentemente, insatisfação do cliente, reclamações e retrabalhos.</t>
-    </r>
-  </si>
-  <si>
-    <t>Desenvolver testes gradativamente durante a iteração.</t>
-  </si>
-  <si>
-    <t>Organizacional</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -514,6 +469,7 @@
     </r>
     <r>
       <rPr>
+        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -524,7 +480,6 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -541,35 +496,24 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> Softwares</t>
+      <t> Softwares) Indisponíveis</t>
     </r>
+  </si>
+  <si>
+    <t>Atraso, ou até não entrega, de sistema.</t>
+  </si>
+  <si>
+    <t>Baixo</t>
+  </si>
+  <si>
+    <t>Máquina de algum membro da equipe de desenvolvimento apresenta problemas.</t>
+  </si>
+  <si>
+    <t>Durante o planejamento inicial, levantar quantidade e qualidade de recursos necessários.</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>) Indisponíveis</t>
-    </r>
-  </si>
-  <si>
-    <t>Atraso, ou até não entrega, de sistema.</t>
-  </si>
-  <si>
-    <t>Baixo</t>
-  </si>
-  <si>
-    <t>Máquina de algum membro da equipe de desenvolvimento apresenta problemas.</t>
-  </si>
-  <si>
-    <t>Durante o planejamento inicial, levantar quantidade e qualidade de recursos necessários.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -580,6 +524,7 @@
     </r>
     <r>
       <rPr>
+        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -590,7 +535,6 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -607,26 +551,15 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Release </t>
+      <t>Release Disponibilizada ao Cliente</t>
     </r>
+  </si>
+  <si>
+    <t>Aumento de escopo iteração atual, aumento de custo referente a disponibilização de tempo.</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Disponibilizada ao Cliente</t>
-    </r>
-  </si>
-  <si>
-    <t>Aumento de escopo iteração atual, aumento de custo referente a disponibilização de tempo.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -643,23 +576,12 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>release </t>
+      <t>release mal realizados.</t>
     </r>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>mal realizados.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -676,29 +598,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>release</t>
+      <t>release.</t>
     </r>
+  </si>
+  <si>
+    <t>Externo</t>
+  </si>
+  <si>
+    <t>Indisponibilidade dos Clientes</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Externo</t>
-  </si>
-  <si>
-    <t>Indisponibilidade dos Clientes</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -715,119 +626,108 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>backlog</t>
+      <t>backlog.</t>
     </r>
+  </si>
+  <si>
+    <t>Cliente se ausenta do Campus por motivos pessoais, profissionais ou de saúde.</t>
+  </si>
+  <si>
+    <t>marcar, de forma antecipada, reuniões e encontros com as clientes.</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Adição de Novos Requisitos</t>
+  </si>
+  <si>
+    <t>Aumento de complexidade de sistema, modificação em escopo inicialmente planejado, aumento de trabalho.</t>
+  </si>
+  <si>
+    <t>Entrada de novo Stakeholder.</t>
+  </si>
+  <si>
+    <t>FALTA RESOLVER DAQUI PARA BAIXO.</t>
+  </si>
+  <si>
+    <t>Mudança em Requisitos</t>
+  </si>
+  <si>
+    <t>Mudança em escopos de iterações já planejadas, provável atraso na finalização de iterações devido o aumento do escopo.</t>
+  </si>
+  <si>
+    <t>Cliente solicitar mudança por conta de novo regimento no Campus.</t>
+  </si>
+  <si>
+    <t>Analisar alteração de escopo e tempo, notificar cliente sobre consequências e implementá-las caso sejam viabilizadas.</t>
+  </si>
+  <si>
+    <t>Necessidade de Utilização para Nova Tecnologia não Planejada pela Equipe</t>
+  </si>
+  <si>
+    <t>Atrasos em iterações, mau uso de tecnologia devido a falta de tempo.</t>
+  </si>
+  <si>
+    <t>Aceitar</t>
+  </si>
+  <si>
+    <t>Inserção de nova ferrramenta não planejada pela equipe durante a ocorrência de uma iteração.</t>
+  </si>
+  <si>
+    <t>Planejar horário fora do planejado para iteração com o intuíto de estudar sobre a ferramenta, mantendo a entrega ainda dentro dos parâmetros.</t>
+  </si>
+  <si>
+    <t>Gerente de Configuração</t>
+  </si>
+  <si>
+    <t>Dificuldade na Utilização de alguma Tecnologia pela Equipe</t>
+  </si>
+  <si>
+    <t>Aumento de escopo de iterações e, consequentemente, atrasos na entrega, baixa qualidade do produto.</t>
+  </si>
+  <si>
+    <t>Utilização de nova ferramenta dificultada por baixa quantidade de documentação da mesma.</t>
+  </si>
+  <si>
+    <t>Verificar a possibilidade de troca de ferramenta sem que a entrega seja afetada.</t>
+  </si>
+  <si>
+    <t>Afastamento de Membro de Equipe por Viagem a Congressos, Concursos e etc.</t>
+  </si>
+  <si>
+    <t>Sobrecarga de trabalho para membro restante, provável atraso ou não finalização de iteração, provável baixa qualidade em entregas.</t>
+  </si>
+  <si>
+    <t>Participação de algum membro da equipe de eventos da área de TI.</t>
+  </si>
+  <si>
+    <t>Buscar erradicação de risco ainda no planejamento de iteração, afim de realizar planejamento de iteração com menos tempo disponível.</t>
+  </si>
+  <si>
+    <t>Afastamento de Membro de Equipe por Motivos de Saúde</t>
+  </si>
+  <si>
+    <t>Algum membro da equipe ser infectado por Zica, Denge ou Chikungunya.</t>
+  </si>
+  <si>
+    <t>Dificuldade de Comunicação entre Membros de Equipe</t>
+  </si>
+  <si>
+    <t>Retrabalho, insconsistência em trabalho produzido.</t>
+  </si>
+  <si>
+    <t>Deslocamento dos membros da equipe para sua cidade natal.</t>
+  </si>
+  <si>
+    <t>Realizar atividades planejadas de forma remota.</t>
+  </si>
+  <si>
+    <t>Desistência de um Membro da Equipe</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Cliente se ausenta do Campus por motivos pessoais, profissionais ou de saúde.</t>
-  </si>
-  <si>
-    <t>marcar, de forma antecipada, reuniões e encontros com as clientes.</t>
-  </si>
-  <si>
-    <t>Clientes</t>
-  </si>
-  <si>
-    <t>Adição de Novos Requisitos</t>
-  </si>
-  <si>
-    <t>Aumento de complexidade de sistema, modificação em escopo inicialmente planejado, aumento de trabalho.</t>
-  </si>
-  <si>
-    <t>Entrada de novo Stakeholder.</t>
-  </si>
-  <si>
-    <t>FALTA RESOLVER DAQUI PARA BAIXO.</t>
-  </si>
-  <si>
-    <t>Mudança em Requisitos</t>
-  </si>
-  <si>
-    <t>Mudança em escopos de iterações já planejadas, provável atraso na finalização de iterações devido o aumento do escopo.</t>
-  </si>
-  <si>
-    <t>Cliente solicitar mudança por conta de novo regimento no Campus.</t>
-  </si>
-  <si>
-    <t>Analisar alteração de escopo e tempo, notificar cliente sobre consequências e implementá-las caso sejam viabilizadas.</t>
-  </si>
-  <si>
-    <t>Necessidade de Utilização para Nova Tecnologia não Planejada pela Equipe</t>
-  </si>
-  <si>
-    <t>Atrasos em iterações, mau uso de tecnologia devido a falta de tempo.</t>
-  </si>
-  <si>
-    <t>Aceitar</t>
-  </si>
-  <si>
-    <t>Inserção de nova ferrramenta não planejada pela equipe durante a ocorrência de uma iteração.</t>
-  </si>
-  <si>
-    <t>Planejar horário fora do planejado para iteração com o intuíto de estudar sobre a ferramenta, mantendo a entrega ainda dentro dos parâmetros.</t>
-  </si>
-  <si>
-    <t>Gerente de Configuração</t>
-  </si>
-  <si>
-    <t>Dificuldade na Utilização de alguma Tecnologia pela Equipe</t>
-  </si>
-  <si>
-    <t>Aumento de escopo de iterações e, consequentemente, atrasos na entrega, baixa qualidade do produto.</t>
-  </si>
-  <si>
-    <t>Utilização de nova ferramenta dificultada por baixa quantidade de documentação da mesma.</t>
-  </si>
-  <si>
-    <t>Verificar a possibilidade de troca de ferramenta sem que a entrega seja afetada.</t>
-  </si>
-  <si>
-    <t>Afastamento de Membro de Equipe por Viagem a Congressos, Concursos e etc.</t>
-  </si>
-  <si>
-    <t>Sobrecarga de trabalho para membro restante, provável atraso ou não finalização de iteração, provável baixa qualidade em entregas.</t>
-  </si>
-  <si>
-    <t>Participação de algum membro da equipe de eventos da área de TI.</t>
-  </si>
-  <si>
-    <t>Buscar erradicação de risco ainda no planejamento de iteração, afim de realizar planejamento de iteração com menos tempo disponível.</t>
-  </si>
-  <si>
-    <t>Afastamento de Membro de Equipe por Motivos de Saúde</t>
-  </si>
-  <si>
-    <t>Algum membro da equipe ser infectado por Zica, Denge ou Chikungunya.</t>
-  </si>
-  <si>
-    <t>Dificuldade de Comunicação entre Membros de Equipe</t>
-  </si>
-  <si>
-    <t>Retrabalho, insconsistência em trabalho produzido.</t>
-  </si>
-  <si>
-    <t>Deslocamento dos membros da equipe para sua cidade natal.</t>
-  </si>
-  <si>
-    <t>Realizar atividades planejadas de forma remota.</t>
-  </si>
-  <si>
-    <t>Desistência de um Membro da Equipe</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -844,38 +744,27 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>releases</t>
+      <t>releases, itens de backlog e produto final, provável baixa qualidade em entregas.</t>
     </r>
+  </si>
+  <si>
+    <t>Desistência do curso de algum membro da equipe.</t>
+  </si>
+  <si>
+    <t>Deslocamento das atividades para os membros restantes, buscar substituto, redefinir escopo.</t>
+  </si>
+  <si>
+    <t>Dificuldade no Acesso ao Sistema Acadêmico do IFPB - Campus Monteiro</t>
+  </si>
+  <si>
+    <t>Atraso de iteração ou inviabilização de funcionalidade referente ao login.</t>
+  </si>
+  <si>
+    <t>Link de ferramenta fora do ar.</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>, itens de backlog e produto final, provável baixa qualidade em entregas.</t>
-    </r>
-  </si>
-  <si>
-    <t>Desistência do curso de algum membro da equipe.</t>
-  </si>
-  <si>
-    <t>Deslocamento das atividades para os membros restantes, buscar substituto, redefinir escopo.</t>
-  </si>
-  <si>
-    <t>Dificuldade no Acesso ao Sistema Acadêmico do IFPB - Campus Monteiro</t>
-  </si>
-  <si>
-    <t>Atraso de iteração ou inviabilização de funcionalidade referente ao login.</t>
-  </si>
-  <si>
-    <t>Link de ferramenta fora do ar.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -892,41 +781,30 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>backlog, </t>
+      <t>backlog, renegociação com cliente sobre entrega de requisito.</t>
     </r>
+  </si>
+  <si>
+    <t>Dificuldade no Acesso a Plataforma SUAP</t>
+  </si>
+  <si>
+    <t>Dificuldade no Acesso ao IceScrum</t>
+  </si>
+  <si>
+    <t>Falha no gerenciamento de iteração.</t>
+  </si>
+  <si>
+    <t>Gerar, sempre que passível de atenção, arquivo .pdf com atividades atualizadas da ferramenta.</t>
+  </si>
+  <si>
+    <t>Líder do Projeto</t>
+  </si>
+  <si>
+    <t>Dificuldade no Acesso ao Jenkis</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>renegociação com cliente sobre entrega de requisito.</t>
-    </r>
-  </si>
-  <si>
-    <t>Dificuldade no Acesso a Plataforma SUAP</t>
-  </si>
-  <si>
-    <t>Dificuldade no Acesso ao IceScrum</t>
-  </si>
-  <si>
-    <t>Falha no gerenciamento de iteração.</t>
-  </si>
-  <si>
-    <t>Gerar, sempre que passível de atenção, arquivo .pdf com atividades atualizadas da ferramenta.</t>
-  </si>
-  <si>
-    <t>Líder do Projeto</t>
-  </si>
-  <si>
-    <t>Dificuldade no Acesso ao Jenkis</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -943,21 +821,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>build</t>
+      <t>build do projeto.</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> do projeto.</t>
-    </r>
   </si>
   <si>
     <t>Deslocar responsabilidade de verificação para algum membro da equipe.</t>
+  </si>
+  <si>
+    <t>Distância de membros da Iterative por conta do carnaval</t>
+  </si>
+  <si>
+    <t>Realizar acompanhamento de membros online</t>
+  </si>
+  <si>
+    <t>TCC</t>
   </si>
   <si>
     <t>Tabela de Severidade</t>
@@ -970,13 +847,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="[$R$-416]\ #,##0.00;[RED]\-[$R$-416]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -998,82 +874,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000080"/>
-      <name val="Arial1"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Black"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF800000"/>
-      <name val="SimSun"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFE6E6FF"/>
-      <name val="SimSun"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1112,6 +912,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial1"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1177,7 +984,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1186,8 +993,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEB613D"/>
-        <bgColor rgb="FFFF8080"/>
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF94BD5E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6E6"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33B299"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -1204,32 +1029,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor rgb="FF94BD5E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6E6"/>
-        <bgColor rgb="FFE6E6FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF33B299"/>
-        <bgColor rgb="FF33CCCC"/>
+        <fgColor rgb="FFEB613D"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -1352,7 +1153,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1376,389 +1177,129 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1766,234 +1307,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="1" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="1" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="1" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="1" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="1" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="2" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="3" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="8" borderId="4" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="8" borderId="5" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="8" borderId="6" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="9" borderId="7" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="8" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="9" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="10" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="108">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="cf1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf1 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf10" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf11" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf12" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf13" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf14" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf15" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf16" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf17" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf18" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf19" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf2" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf2 2" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf20" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf21" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf22" xfId="36" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf23" xfId="37" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf24" xfId="38" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf25" xfId="39" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf26" xfId="40" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf27" xfId="41" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf28" xfId="42" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf29" xfId="43" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf3" xfId="44" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf3 2" xfId="45" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf30" xfId="46" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf4" xfId="47" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf4 2" xfId="48" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf5" xfId="49" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf5 2" xfId="50" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf6" xfId="51" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf6 2" xfId="52" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf7" xfId="53" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf7 2" xfId="54" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf8" xfId="55" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf8 2" xfId="56" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="cf9" xfId="57" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="58" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="59" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 2" xfId="60" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 3" xfId="61" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Norm??" xfId="62" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Norm?? 2" xfId="63" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 2" xfId="64" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 4" xfId="65" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 2" xfId="66" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 5" xfId="67" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título1" xfId="68" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título1 2" xfId="69" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título10" xfId="70" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título10 2" xfId="71" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título11" xfId="72" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título11 2" xfId="73" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título12" xfId="74" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título12 2" xfId="75" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título13" xfId="76" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título13 2" xfId="77" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título14" xfId="78" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título14 2" xfId="79" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título15" xfId="80" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título15 2" xfId="81" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título16" xfId="82" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título16 2" xfId="83" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título17" xfId="84" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título17 2" xfId="85" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título18" xfId="86" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título18 2" xfId="87" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título19" xfId="88" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título19 2" xfId="89" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título2" xfId="90" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título2 2" xfId="91" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título20" xfId="92" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título20 2" xfId="93" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título21" xfId="94" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título21 2" xfId="95" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título22" xfId="96" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título22 2" xfId="97" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título23" xfId="98" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título23 2" xfId="99" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título24" xfId="100" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título24 2" xfId="101" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título25" xfId="102" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título25 2" xfId="103" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título26" xfId="104" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título26 2" xfId="105" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título27" xfId="106" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título27 2" xfId="107" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título3" xfId="108" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título3 2" xfId="109" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título4" xfId="110" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título4 2" xfId="111" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título5" xfId="112" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título5 2" xfId="113" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título6" xfId="114" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título6 2" xfId="115" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título7" xfId="116" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título7 2" xfId="117" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título8" xfId="118" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título8 2" xfId="119" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título9" xfId="120" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Sem título9 2" xfId="121" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -2014,13 +1345,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEB613D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF94BD5E"/>
         </patternFill>
       </fill>
@@ -2032,6 +1356,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF94BD5E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEB613D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2076,41 +1407,6 @@
         <color rgb="FF000080"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEB613D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEB613D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF94BD5E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -2133,7 +1429,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFE6E6E6"/>
-      <rgbColor rgb="FFE6E6FF"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -2180,15 +1476,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>179280</xdr:colOff>
+      <xdr:colOff>206280</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>678600</xdr:colOff>
+      <xdr:colOff>705240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2201,8 +1497,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="607680" y="57600"/>
-          <a:ext cx="499320" cy="674640"/>
+          <a:off x="634680" y="48600"/>
+          <a:ext cx="498960" cy="674280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2224,25 +1520,25 @@
   </sheetPr>
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E9" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.82186234817814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.4898785425101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.0647773279352"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.8097165991903"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.3846153846154"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -2382,7 +1678,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" s="7" customFormat="true" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="6" customFormat="true" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2397,61 +1693,61 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" s="10" customFormat="true" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+    <row r="10" s="9" customFormat="true" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" s="7" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
+    <row r="11" s="6" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="14" t="s">
@@ -2460,40 +1756,40 @@
       <c r="G11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="13" t="s">
+      <c r="M11" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" s="7" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
+    <row r="12" s="6" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="n">
         <f aca="false">A11+1</f>
         <v>2</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="14" t="s">
@@ -2502,40 +1798,40 @@
       <c r="G12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="M12" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" s="7" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="n">
+    <row r="13" s="6" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="n">
         <f aca="false">A12+1</f>
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="14" t="s">
@@ -2544,40 +1840,40 @@
       <c r="G13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" s="7" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="n">
+    <row r="14" s="6" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="n">
         <f aca="false">A13+1</f>
         <v>4</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="14" t="s">
@@ -2586,40 +1882,40 @@
       <c r="G14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="M14" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" s="7" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="n">
+    <row r="15" s="6" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="n">
         <f aca="false">A14+1</f>
         <v>5</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F15" s="14" t="s">
@@ -2628,40 +1924,40 @@
       <c r="G15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" s="7" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="n">
+    <row r="16" s="6" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="n">
         <f aca="false">A15+1</f>
         <v>6</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="14" t="s">
@@ -2670,40 +1966,40 @@
       <c r="G16" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="M16" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" s="7" customFormat="true" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="n">
+    <row r="17" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="n">
         <f aca="false">A16+1</f>
         <v>7</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>60</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -2712,40 +2008,40 @@
       <c r="G17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="13" t="s">
+      <c r="M17" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" s="7" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="n">
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="n">
         <f aca="false">A17+1</f>
         <v>8</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>65</v>
       </c>
       <c r="F18" s="14" t="s">
@@ -2754,40 +2050,40 @@
       <c r="G18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="L18" s="12" t="s">
+      <c r="L18" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="M18" s="13" t="s">
+      <c r="M18" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" s="7" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="n">
+    <row r="19" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="n">
         <f aca="false">A18+1</f>
         <v>9</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>70</v>
       </c>
       <c r="F19" s="14" t="s">
@@ -2796,40 +2092,40 @@
       <c r="G19" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="L19" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" s="7" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="n">
+    <row r="20" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="n">
         <f aca="false">A19+1</f>
         <v>10</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>74</v>
       </c>
       <c r="F20" s="14" t="s">
@@ -2838,40 +2134,40 @@
       <c r="G20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L20" s="12" t="s">
+      <c r="L20" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="M20" s="13" t="s">
+      <c r="M20" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" s="7" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="n">
+    <row r="21" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="n">
         <f aca="false">A20+1</f>
         <v>11</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>78</v>
       </c>
       <c r="F21" s="14" t="s">
@@ -2880,40 +2176,40 @@
       <c r="G21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J21" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="M21" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" s="7" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="n">
+    <row r="22" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="n">
         <f aca="false">A21+1</f>
         <v>12</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="11" t="s">
         <v>84</v>
       </c>
       <c r="F22" s="14" t="s">
@@ -2922,40 +2218,40 @@
       <c r="G22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="L22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="M22" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="n">
+      <c r="A23" s="10" t="n">
         <f aca="false">A22+1</f>
         <v>13</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>88</v>
       </c>
       <c r="F23" s="14" t="s">
@@ -2964,40 +2260,40 @@
       <c r="G23" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J23" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="K23" s="12" t="s">
+      <c r="K23" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L23" s="12" t="s">
+      <c r="L23" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="M23" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" s="7" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="n">
+    <row r="24" s="6" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="n">
         <f aca="false">A23+1</f>
         <v>14</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>88</v>
       </c>
       <c r="F24" s="14" t="s">
@@ -3006,40 +2302,40 @@
       <c r="G24" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="K24" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M24" s="13" t="s">
+      <c r="M24" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" s="7" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="n">
+    <row r="25" s="6" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="n">
         <f aca="false">A24+1</f>
         <v>15</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
         <v>94</v>
       </c>
       <c r="F25" s="14" t="s">
@@ -3048,40 +2344,40 @@
       <c r="G25" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="J25" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="L25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M25" s="13" t="s">
+      <c r="M25" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" s="7" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="n">
+    <row r="26" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="n">
         <f aca="false">A25+1</f>
         <v>16</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="13" t="s">
         <v>98</v>
       </c>
       <c r="F26" s="14" t="s">
@@ -3090,40 +2386,40 @@
       <c r="G26" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J26" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="K26" s="17" t="s">
+      <c r="K26" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="L26" s="12" t="s">
+      <c r="L26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="M26" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="n">
+      <c r="A27" s="10" t="n">
         <f aca="false">A26+1</f>
         <v>17</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>102</v>
       </c>
       <c r="F27" s="14" t="s">
@@ -3132,40 +2428,40 @@
       <c r="G27" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="I27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="J27" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="K27" s="12" t="s">
+      <c r="K27" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="L27" s="12" t="s">
+      <c r="L27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M27" s="13" t="s">
+      <c r="M27" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="n">
+      <c r="A28" s="10" t="n">
         <f aca="false">A27+1</f>
         <v>18</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="11" t="s">
         <v>102</v>
       </c>
       <c r="F28" s="14" t="s">
@@ -3174,40 +2470,40 @@
       <c r="G28" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="L28" s="12" t="s">
+      <c r="L28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M28" s="13" t="s">
+      <c r="M28" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="n">
+      <c r="A29" s="10" t="n">
         <f aca="false">A28+1</f>
         <v>19</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="11" t="s">
         <v>107</v>
       </c>
       <c r="F29" s="14" t="s">
@@ -3216,37 +2512,37 @@
       <c r="G29" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="I29" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="J29" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K29" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="L29" s="17" t="s">
+      <c r="L29" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="M29" s="13" t="s">
+      <c r="M29" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="n">
+      <c r="A30" s="10" t="n">
         <f aca="false">A29+1</f>
         <v>20</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="18" t="s">
         <v>110</v>
       </c>
       <c r="E30" s="19" t="s">
@@ -3258,22 +2554,22 @@
       <c r="G30" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="L30" s="17" t="s">
+      <c r="L30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="M30" s="13" t="s">
+      <c r="M30" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3281,16 +2577,25 @@
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="21"/>
+      <c r="D31" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="E31" s="21"/>
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
       <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
+      <c r="K31" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="L31" s="21"/>
       <c r="M31" s="22"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="49.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="49.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3360,17 +2665,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G44">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"Alto"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F44">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"Baixa"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H44">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"Baixa"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3453,20 +2758,20 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3484,7 +2789,7 @@
     </row>
     <row r="3" customFormat="false" ht="44.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="28" t="s">
@@ -3548,29 +2853,9 @@
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:A6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:D4,C5">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"Alta"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4,D5:E5,C6:E6">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>"Alta"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C4:E6">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"Baixa"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:D4,C5">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>"Média"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4,D5:E5,C6:E6">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>"Média"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>